<commit_message>
project update & refactored code
Added a graphical user interface (GUI) using Java Swing for better interaction.
Refactored existing code for improved readability and maintainability.
Added detailed comments to enhance code documentation and understanding.
</commit_message>
<xml_diff>
--- a/Search_Algorithms_Project/lib/bin/main/data_output/SequentialExecutionTimes.xlsx
+++ b/Search_Algorithms_Project/lib/bin/main/data_output/SequentialExecutionTimes.xlsx
@@ -4243,7 +4243,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H1048576"/>
@@ -4366,11 +4366,51 @@
       </c>
     </row>
     <row r="5">
-      <c r="E5" t="n">
-        <v>0.0095471</v>
+      <c r="C5" t="n">
+        <v>0.0199743</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.0019937</v>
+      <c r="D5" t="n">
+        <v>0.0026535</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="n">
+        <v>0.0177186</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0048243</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="n">
+        <v>0.0057744</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0062909</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="n">
+        <v>0.0188013</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0033218</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="n">
+        <v>0.019903</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0026143</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="n">
+        <v>0.0199379</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0042961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>